<commit_message>
success task Arif 0902_7 filename 90.0498
</commit_message>
<xml_diff>
--- a/Arif 0902_7/Arif 0902_7.xlsx
+++ b/Arif 0902_7/Arif 0902_7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0902_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F480242F-BD64-457E-980F-76999EBA7D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B32250B-C561-4A77-9B28-0466DA069C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
   <si>
     <r>
       <rPr>
@@ -283,7 +283,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,15 +339,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -359,6 +350,31 @@
       <color rgb="FFFF0000"/>
       <name val="Eurostile"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -419,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -459,16 +475,13 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,6 +495,27 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,19 +1008,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="20" customWidth="1"/>
     <col min="5" max="5" width="66.85546875" customWidth="1"/>
     <col min="6" max="6" width="56.7109375" customWidth="1"/>
-    <col min="7" max="9" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.5703125" customWidth="1"/>
+    <col min="8" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -1021,8 +1056,8 @@
       <c r="B2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="11" t="s">
         <v>12</v>
       </c>
@@ -1044,8 +1079,8 @@
       <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
       <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
@@ -1067,8 +1102,8 @@
       <c r="B4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
       <c r="E4" s="11" t="s">
         <v>19</v>
       </c>
@@ -1090,8 +1125,8 @@
       <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="11" t="s">
         <v>19</v>
       </c>
@@ -1113,8 +1148,8 @@
       <c r="B6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
       <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
@@ -1136,8 +1171,8 @@
       <c r="B7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="11" t="s">
         <v>25</v>
       </c>
@@ -1157,8 +1192,8 @@
       <c r="B8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="11" t="s">
         <v>28</v>
       </c>
@@ -1171,30 +1206,30 @@
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" s="16" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A9" s="13">
+    <row r="9" spans="1:9" s="27" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A9" s="23">
         <v>90.049599999999998</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="19">
+      <c r="C9" s="25">
         <v>281</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
     </row>
     <row r="10" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
       <c r="A10" s="10">
@@ -1203,8 +1238,8 @@
       <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="9" t="s">
         <v>30</v>
       </c>
@@ -1221,26 +1256,30 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A11" s="10">
+    <row r="11" spans="1:9" s="27" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A11" s="23">
         <v>90.049800000000005</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="11" t="s">
+      <c r="C11" s="25">
+        <v>68</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
     </row>
     <row r="12" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
       <c r="A12" s="10">
@@ -1249,9 +1288,9 @@
       <c r="B12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="11" t="s">
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="9" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="11" t="s">
@@ -1261,28 +1300,28 @@
         <v>39</v>
       </c>
       <c r="H12" s="11"/>
-      <c r="I12" s="17"/>
-    </row>
-    <row r="13" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A13" s="10">
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" s="15" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A13" s="13">
         <v>90.051000000000002</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="11" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
       <c r="A14" s="10">
@@ -1291,9 +1330,9 @@
       <c r="B14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="11" t="s">
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="9" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="11" t="s">
@@ -1310,9 +1349,9 @@
       <c r="B15" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="11" t="s">
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="9" t="s">
         <v>47</v>
       </c>
       <c r="F15" s="11" t="s">
@@ -1331,15 +1370,15 @@
       <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="11" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="9" t="s">
         <v>50</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>51</v>
       </c>
       <c r="H16" s="11" t="s">
@@ -1354,9 +1393,9 @@
       <c r="B17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="11" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="9" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="11" t="s">
@@ -1375,9 +1414,9 @@
       <c r="B18" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="11" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="9" t="s">
         <v>56</v>
       </c>
       <c r="F18" s="11" t="s">
@@ -1394,8 +1433,8 @@
       <c r="B19" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="11" t="s">
         <v>59</v>
       </c>
@@ -1413,8 +1452,8 @@
       <c r="B20" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="11" t="s">
         <v>61</v>
       </c>
@@ -1434,8 +1473,8 @@
       <c r="B21" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="11" t="s">
         <v>64</v>
       </c>
@@ -1449,8 +1488,8 @@
     <row r="22" spans="1:9">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -1462,8 +1501,16 @@
     <hyperlink ref="E9" r:id="rId1" xr:uid="{555C19E9-7972-42D2-B98E-4F969C399866}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{809A3FBA-31DF-40C3-87EA-94C34F11ED70}"/>
     <hyperlink ref="E10" r:id="rId3" xr:uid="{49442610-B812-4A01-A3E9-CD41577F7FA4}"/>
+    <hyperlink ref="E11" r:id="rId4" xr:uid="{6F076A57-CEBB-4B75-AE7C-471F69658278}"/>
+    <hyperlink ref="E12" r:id="rId5" xr:uid="{3D44EC1C-5319-4E06-A4E6-4E39B0769948}"/>
+    <hyperlink ref="E13" r:id="rId6" xr:uid="{CEDF2FDD-6F7A-49EF-B8C8-70F1A3AEF09B}"/>
+    <hyperlink ref="E14" r:id="rId7" xr:uid="{43BF7CB6-B10C-4B83-88EC-377030D6B1B7}"/>
+    <hyperlink ref="E15" r:id="rId8" display="https://www.bde.es/bde/en/secciones/servicios/Particulares_y_e/registro-de-proveedores-de-servicios-de-cambio-de-moneda-virtual-por-moneda-fiduciaria-y-de-custodia-de-monederos-electronicos/registro-de-proveedores-de-servicios-de-cambio-de-moneda-virtual-por-moneda-fiduciaria-y-de-custodia-de-monederos-electronicos.html" xr:uid="{5ACF4882-4D9A-4C8D-A091-897E79099E14}"/>
+    <hyperlink ref="E16" r:id="rId9" xr:uid="{0CA5F505-CAC6-4F44-9535-4FC318622D7E}"/>
+    <hyperlink ref="E17" r:id="rId10" xr:uid="{6126EE96-B80D-4A7B-87FC-FE702ED5D54A}"/>
+    <hyperlink ref="E18" r:id="rId11" xr:uid="{D62B8002-1270-4E16-8490-15EADB6C88C7}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
succes task Arif_12(Prio2k) filename 90.0783
</commit_message>
<xml_diff>
--- a/Arif 0902_7/Arif 0902_7.xlsx
+++ b/Arif 0902_7/Arif 0902_7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0902_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B32250B-C561-4A77-9B28-0466DA069C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF1404-ECE0-4C0A-867E-2928FF5E4F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -515,6 +515,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1008,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1173,7 +1185,7 @@
       </c>
       <c r="C7" s="16"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="11" t="s">
@@ -1302,26 +1314,26 @@
       <c r="H12" s="11"/>
       <c r="I12" s="16"/>
     </row>
-    <row r="13" spans="1:9" s="15" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A13" s="13">
+    <row r="13" spans="1:9" s="32" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A13" s="29">
         <v>90.051000000000002</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="22" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="30"/>
+      <c r="H13" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="14"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
       <c r="A14" s="10">
@@ -1407,24 +1419,24 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A18" s="10">
+    <row r="18" spans="1:9" s="15" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A18" s="13">
         <v>90.051900000000003</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="9" t="s">
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
       <c r="A19" s="10">
@@ -1435,7 +1447,7 @@
       </c>
       <c r="C19" s="16"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="9" t="s">
         <v>59</v>
       </c>
       <c r="F19" s="11" t="s">
@@ -1454,7 +1466,7 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="9" t="s">
         <v>61</v>
       </c>
       <c r="F20" s="11" t="s">
@@ -1475,7 +1487,7 @@
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="9" t="s">
         <v>64</v>
       </c>
       <c r="F21" s="11" t="s">
@@ -1509,8 +1521,12 @@
     <hyperlink ref="E16" r:id="rId9" xr:uid="{0CA5F505-CAC6-4F44-9535-4FC318622D7E}"/>
     <hyperlink ref="E17" r:id="rId10" xr:uid="{6126EE96-B80D-4A7B-87FC-FE702ED5D54A}"/>
     <hyperlink ref="E18" r:id="rId11" xr:uid="{D62B8002-1270-4E16-8490-15EADB6C88C7}"/>
+    <hyperlink ref="E19" r:id="rId12" xr:uid="{5328BC9E-0DC1-4D7A-83E6-F6993CA916E8}"/>
+    <hyperlink ref="E20" r:id="rId13" xr:uid="{7E1C440B-DC70-4BA6-82E3-9B691A72DD8E}"/>
+    <hyperlink ref="E21" r:id="rId14" xr:uid="{4C0820DC-0B5A-4066-8134-F2D68E7F6BC5}"/>
+    <hyperlink ref="E7" r:id="rId15" xr:uid="{DED9C6FB-D78D-444C-AA6B-050CE6E83CB7}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
success task Arif 0902_7 filename 90.0519
</commit_message>
<xml_diff>
--- a/Arif 0902_7/Arif 0902_7.xlsx
+++ b/Arif 0902_7/Arif 0902_7.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Scraping\Don Osterloh\Scraping data\Arif 0902_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF1404-ECE0-4C0A-867E-2928FF5E4F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DAF937-E333-45BE-8707-76474249DBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="66">
   <si>
     <r>
       <rPr>
@@ -273,17 +284,18 @@
     <t>https://www.regafi.fr/spip.php?page=results&amp;type=advanced&amp;id_secteur=3&amp;lang=en&amp;denomination=&amp;siren=&amp;cib=&amp;bic=&amp;nom=&amp;siren_agent=&amp;num=&amp;cat=01-TBR07&amp;retrait=0</t>
   </si>
   <si>
-    <t>Sep 03 2023</t>
+    <t>No avaliable  data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000_);[Red]\(0.0000\)"/>
+    <numFmt numFmtId="170" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,8 +388,73 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Eurostile"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Eurostile"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,7 +518,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -469,36 +552,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -528,6 +587,84 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1021,15 +1158,15 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="14"/>
+    <col min="2" max="2" width="18.85546875" style="44" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="93.5703125" customWidth="1"/>
     <col min="5" max="5" width="66.85546875" customWidth="1"/>
     <col min="6" max="6" width="56.7109375" customWidth="1"/>
     <col min="7" max="7" width="44.5703125" customWidth="1"/>
@@ -1037,14 +1174,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
       <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1062,15 +1197,15 @@
       </c>
     </row>
     <row r="2" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="10">
+      <c r="A2" s="33"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="10">
         <v>90.048900000000003</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F2" s="11" t="s">
@@ -1085,14 +1220,14 @@
       <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A3" s="10">
+      <c r="A3" s="33"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="10">
         <v>90.049000000000007</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
       <c r="E3" s="11" t="s">
         <v>12</v>
       </c>
@@ -1108,14 +1243,14 @@
       <c r="I3" s="11"/>
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="33"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="10">
         <v>90.049099999999996</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
       <c r="E4" s="11" t="s">
         <v>19</v>
       </c>
@@ -1131,14 +1266,14 @@
       <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="33"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="10">
         <v>90.049199999999999</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
       <c r="E5" s="11" t="s">
         <v>19</v>
       </c>
@@ -1154,14 +1289,14 @@
       <c r="I5" s="11"/>
     </row>
     <row r="6" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A6" s="10">
+      <c r="A6" s="33"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="10">
         <v>90.049300000000002</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
       <c r="E6" s="9" t="s">
         <v>19</v>
       </c>
@@ -1177,14 +1312,14 @@
       <c r="I6" s="11"/>
     </row>
     <row r="7" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="33"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="10">
         <v>90.049400000000006</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
       <c r="E7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1198,15 +1333,15 @@
       <c r="I7" s="11"/>
     </row>
     <row r="8" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="33"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="10">
         <v>90.049499999999995</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -1218,40 +1353,40 @@
       </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" spans="1:9" s="27" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A9" s="23">
+    <row r="9" spans="1:9" s="19" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A9" s="34">
+        <v>281</v>
+      </c>
+      <c r="B9" s="46">
+        <v>45172</v>
+      </c>
+      <c r="C9" s="15">
         <v>90.049599999999998</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="D9" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25">
-        <v>281</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="24" t="s">
+      <c r="F9" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A10" s="10">
+      <c r="A10" s="33"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="10">
         <v>90.049700000000001</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="21"/>
       <c r="E10" s="9" t="s">
         <v>30</v>
       </c>
@@ -1268,145 +1403,145 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="27" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A11" s="23">
+    <row r="11" spans="1:9" s="19" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A11" s="34">
+        <v>68</v>
+      </c>
+      <c r="B11" s="46">
+        <v>45172</v>
+      </c>
+      <c r="C11" s="15">
         <v>90.049800000000005</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="D11" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="25">
-        <v>68</v>
-      </c>
-      <c r="D11" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="E11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="F11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-    </row>
-    <row r="12" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A12" s="10">
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" s="29" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A12" s="35"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="30">
         <v>90.049899999999994</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="D12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="11"/>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" s="32" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A13" s="29">
+      <c r="H12" s="13"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="1:9" s="24" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A13" s="36"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="21">
         <v>90.051000000000002</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="D13" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="31" t="s">
+      <c r="E13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="I13" s="30"/>
-    </row>
-    <row r="14" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A14" s="10">
+      <c r="I13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" s="29" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A14" s="35"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="30">
         <v>90.051500000000004</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="D14" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A15" s="10">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" s="29" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A15" s="35"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="30">
         <v>90.051599999999993</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="D15" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="38" t="s">
         <v>47</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="G15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-    </row>
-    <row r="16" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A16" s="10">
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" s="40" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A16" s="39"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="41">
         <v>90.051699999999997</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="D16" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="I16" s="11"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A17" s="10">
+      <c r="A17" s="33"/>
+      <c r="B17" s="45"/>
+      <c r="C17" s="10">
         <v>90.0518</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
       <c r="E17" s="9" t="s">
         <v>50</v>
       </c>
@@ -1419,89 +1554,103 @@
       </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="1:9" s="15" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A18" s="13">
+    <row r="18" spans="1:9" s="19" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A18" s="17">
+        <v>20175</v>
+      </c>
+      <c r="B18" s="46">
+        <v>45175</v>
+      </c>
+      <c r="C18" s="15">
         <v>90.051900000000003</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="D18" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A19" s="10">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" s="19" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A19" s="17">
+        <v>10</v>
+      </c>
+      <c r="B19" s="46">
+        <v>45175</v>
+      </c>
+      <c r="C19" s="15">
         <v>90.052000000000007</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="D19" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="F19" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A20" s="10">
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" s="25" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A20" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="50">
+        <v>45175</v>
+      </c>
+      <c r="C20" s="26">
         <v>90.052099999999996</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="D20" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="11" t="s">
+      <c r="F20" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="G20" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" spans="1:9" s="12" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A21" s="10">
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+    </row>
+    <row r="21" spans="1:9" s="19" customFormat="1" ht="31.5" customHeight="1">
+      <c r="A21" s="34">
+        <v>879</v>
+      </c>
+      <c r="B21" s="46">
+        <v>45175</v>
+      </c>
+      <c r="C21" s="15">
         <v>90.052199999999999</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="D21" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="11" t="s">
+      <c r="F21" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
@@ -1525,8 +1674,10 @@
     <hyperlink ref="E20" r:id="rId13" xr:uid="{7E1C440B-DC70-4BA6-82E3-9B691A72DD8E}"/>
     <hyperlink ref="E21" r:id="rId14" xr:uid="{4C0820DC-0B5A-4066-8134-F2D68E7F6BC5}"/>
     <hyperlink ref="E7" r:id="rId15" xr:uid="{DED9C6FB-D78D-444C-AA6B-050CE6E83CB7}"/>
+    <hyperlink ref="E2" r:id="rId16" xr:uid="{12512C79-3C12-4D55-86AB-7AA71ADBEE1F}"/>
+    <hyperlink ref="E8" r:id="rId17" xr:uid="{A68F2E53-9DB1-4EA2-91EE-BA6E268BCE8E}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>